<commit_message>
chore: Update master_report.xlsx with 4log.json data
</commit_message>
<xml_diff>
--- a/master_report.xlsx
+++ b/master_report.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Day 1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Day 2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Day 3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Day 4" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -185,12 +186,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$4</f>
+              <f>'Master Summary'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$C$2:$C$4</f>
+              <f>'Master Summary'!$C$2:$C$5</f>
             </numRef>
           </val>
         </ser>
@@ -217,12 +218,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$4</f>
+              <f>'Master Summary'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$D$2:$D$4</f>
+              <f>'Master Summary'!$D$2:$D$5</f>
             </numRef>
           </val>
         </ser>
@@ -249,12 +250,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$4</f>
+              <f>'Master Summary'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$E$2:$E$4</f>
+              <f>'Master Summary'!$E$2:$E$5</f>
             </numRef>
           </val>
         </ser>
@@ -733,6 +734,307 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 4'!B74</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 4'!$A$75:$A$84</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 4'!$B$75:$B$84</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 4'!B86</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 4'!$A$87:$A$96</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 4'!$B$87:$B$96</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 4'!B98</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 4'!$A$99:$A$108</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 4'!$B$99:$B$108</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Hourly Package Retrieval Throughput</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 4'!B110</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 4'!$A$111:$A$113</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 4'!$B$111:$B$113</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Hour of Day</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Packages Retrieved</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
@@ -777,12 +1079,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$4</f>
+              <f>'Master Summary'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$J$2:$J$4</f>
+              <f>'Master Summary'!$J$2:$J$5</f>
             </numRef>
           </val>
         </ser>
@@ -814,7 +1116,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Master Summary'!$K$2:$K$4</f>
+              <f>'Master Summary'!$K$2:$K$5</f>
             </numRef>
           </val>
         </ser>
@@ -1408,7 +1710,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>5</row>
+      <row>6</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1430,7 +1732,7 @@
     <from>
       <col>9</col>
       <colOff>0</colOff>
-      <row>5</row>
+      <row>6</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1710,6 +2012,99 @@
       <col>4</col>
       <colOff>0</colOff>
       <row>73</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>73</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>85</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>97</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>109</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -2019,7 +2414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2221,6 +2616,49 @@
       </c>
       <c r="M4" t="n">
         <v>0.3835713072222222</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-07-08</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>15.04</v>
+      </c>
+      <c r="D5" t="n">
+        <v>25.15</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="F5" t="n">
+        <v>37</v>
+      </c>
+      <c r="G5" t="n">
+        <v>44</v>
+      </c>
+      <c r="H5" t="n">
+        <v>26</v>
+      </c>
+      <c r="I5" t="n">
+        <v>45</v>
+      </c>
+      <c r="J5" t="n">
+        <v>92.95999999999999</v>
+      </c>
+      <c r="K5" t="n">
+        <v>21</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.8232046736111107</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.2797005152777778</v>
       </c>
     </row>
   </sheetData>
@@ -2235,7 +2673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2324,6 +2762,16 @@
           <t>Error message not found</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Failed to execute pick and raise operation: Waypoint execution failed</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Failed to pick and raise</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2430,6 +2878,49 @@
         <v>1</v>
       </c>
       <c r="P4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-07-08</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
+      <c r="N5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" t="n">
+        <v>4</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7136,52 +7627,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Event Label</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Event Label</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Package ID</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Event Label</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
@@ -7902,24 +8393,24 @@
     </row>
     <row r="22"/>
     <row r="23">
-      <c r="B23" s="1" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="E23" s="1" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="J23" s="1" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -7929,7 +8420,7 @@
           <t>13.16</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -7939,7 +8430,7 @@
           <t>24.47</t>
         </is>
       </c>
-      <c r="I24" s="1" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -7951,7 +8442,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>Minimum</t>
         </is>
@@ -7961,7 +8452,7 @@
           <t>8.96</t>
         </is>
       </c>
-      <c r="D25" s="1" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Minimum</t>
         </is>
@@ -7971,7 +8462,7 @@
           <t>16.46</t>
         </is>
       </c>
-      <c r="I25" s="1" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>Minimum</t>
         </is>
@@ -7983,7 +8474,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Maximum</t>
         </is>
@@ -7993,7 +8484,7 @@
           <t>21.71</t>
         </is>
       </c>
-      <c r="D26" s="1" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Maximum</t>
         </is>
@@ -8003,7 +8494,7 @@
           <t>34.15</t>
         </is>
       </c>
-      <c r="I26" s="1" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>Maximum</t>
         </is>
@@ -8016,17 +8507,17 @@
     </row>
     <row r="27"/>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B28" s="1" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>Error Type</t>
         </is>
       </c>
-      <c r="C28" s="1" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
         <is>
           <t>Error Message</t>
         </is>
@@ -8170,12 +8661,12 @@
     </row>
     <row r="37"/>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>Time Bins (s)</t>
         </is>
       </c>
-      <c r="B38" s="1" t="inlineStr">
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -8283,12 +8774,12 @@
     </row>
     <row r="49"/>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
+      <c r="A50" s="2" t="inlineStr">
         <is>
           <t>Time Bins (s)</t>
         </is>
       </c>
-      <c r="B50" s="1" t="inlineStr">
+      <c r="B50" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -8396,12 +8887,12 @@
     </row>
     <row r="61"/>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
+      <c r="A62" s="2" t="inlineStr">
         <is>
           <t>Time Bins (s)</t>
         </is>
       </c>
-      <c r="B62" s="1" t="inlineStr">
+      <c r="B62" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -8509,12 +9000,12 @@
     </row>
     <row r="73"/>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
+      <c r="A74" s="2" t="inlineStr">
         <is>
           <t>Hour</t>
         </is>
       </c>
-      <c r="B74" s="1" t="inlineStr">
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>Packages Retrieved</t>
         </is>
@@ -8545,4 +9036,2490 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N114"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Event Label</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Event Label</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Package ID</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Event Label</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:48:28.689791</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>9.739755708000303</v>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:50:08.726271</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 27)</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>24.89038071800314</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:48:26.002397</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>6.926302025996847</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:52:40.129724</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>12.22106634699958</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:50:08.726271</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 19)</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>28.60336724799708</v>
+      </c>
+      <c r="G3" t="n">
+        <v>19</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:52:36.877685</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>7.405810242998996</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:53:14.619920</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>14.76278409599763</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:44:22.546976</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 12)</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>25.59200767200002</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:53:08.503846</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>7.149856347001332</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:54:00.165943</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>16.64273647500158</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:44:22.546976</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 35)</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>18.74283120600001</v>
+      </c>
+      <c r="G5" t="n">
+        <v>35</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:53:51.746637</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>6.760863604999031</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:54:51.120320</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>23.05658748399946</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:47:43.737777</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 4)</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>32.11041911900003</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:54:42.577184</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>7.368505602000369</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:56:30.098936</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>18.9554138229978</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:47:43.737777</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 32)</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>15.56475010399998</v>
+      </c>
+      <c r="G7" t="n">
+        <v>32</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:56:20.901999</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>6.23434560899841</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:13:04.044103</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>9.254658166999434</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:47:43.737777</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 36)</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>35.30523037399996</v>
+      </c>
+      <c r="G8" t="n">
+        <v>36</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:56:51.535369</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>9.225246816000436</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:13:31.569603</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>12.97762150299968</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:47:43.737777</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 3)</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>25.04282548599997</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:13:02.833150</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>7.862596336999559</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:14:18.808490</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>14.23317721300191</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:47:43.737777</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 24)</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>22.31566797599999</v>
+      </c>
+      <c r="G10" t="n">
+        <v>24</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:13:27.038784</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>6.690923350000958</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:16:17.698058</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>13.04225058299926</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:50:18.044829</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 6)</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>24.246449095</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:14:15.137647</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>6.768257601997902</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:17:26.707028</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>19.01534114300011</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:50:18.044829</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 1)</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>31.50091320000001</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:16:11.156932</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>6.377986020997923</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:18:04.202887</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>13.10294801599957</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:53:09.575278</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 5)</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>25.51722777400005</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:16:49.823491</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>7.915042188000371</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:18:34.966062</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>16.75854314900062</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:53:09.575278</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 14)</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>20.30912766799997</v>
+      </c>
+      <c r="G14" t="n">
+        <v>14</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:17:19.846311</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>6.624801676000061</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:19:56.528242</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>15.07485731100314</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:53:09.575278</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 15)</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>22.10389929199994</v>
+      </c>
+      <c r="G15" t="n">
+        <v>15</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:17:57.047889</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>5.820372376998421</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:20:40.389670</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>18.86117539599945</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:53:09.575278</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 23)</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>19.31567681599995</v>
+      </c>
+      <c r="G16" t="n">
+        <v>23</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:18:27.555767</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>5.817229492000479</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:22:19.657973</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>12.68264764600099</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:53:09.575278</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 16)</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>31.2704850670001</v>
+      </c>
+      <c r="G17" t="n">
+        <v>16</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:19:49.128990</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>6.013141718001862</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:22:49.749577</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>9.223377932998119</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:54:14.897822</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 28)</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>25.20978284599994</v>
+      </c>
+      <c r="G18" t="n">
+        <v>28</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:20:33.492396</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>8.454442474998359</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:23:36.994186</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>11.0098028809989</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:54:14.897822</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 34)</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>19.79026448000002</v>
+      </c>
+      <c r="G19" t="n">
+        <v>34</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:22:12.818347</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>5.707087474998843</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:24:06.914321</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>15.22750738899776</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:56:33.240542</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 25)</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>34.69862186099999</v>
+      </c>
+      <c r="G20" t="n">
+        <v>25</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:22:46.707645</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>6.082853595002234</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:24:43.190367</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>11.83240232900062</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:56:33.240542</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 31)</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>16.14772895400006</v>
+      </c>
+      <c r="G21" t="n">
+        <v>31</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:23:33.814680</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>5.842845523999131</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:25:13.359043</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>12.74872948400298</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:56:33.240542</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 26)</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>37.98819528800004</v>
+      </c>
+      <c r="G22" t="n">
+        <v>26</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:23:59.361414</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>5.987875787999656</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:25:54.201304</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>19.02213804799976</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:56:33.240542</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 33)</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>21.90726079299998</v>
+      </c>
+      <c r="G23" t="n">
+        <v>33</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:24:38.087652</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>6.598010349000106</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:26:34.001276</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>18.50043175099927</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:01:09.468831</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 11)</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>25.71080897299998</v>
+      </c>
+      <c r="G24" t="n">
+        <v>11</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:25:10.315612</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>6.282159440001124</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:27:43.782502</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>13.30749840700082</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:01:09.468831</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 21)</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>19.09752114800017</v>
+      </c>
+      <c r="G25" t="n">
+        <v>21</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:25:44.753682</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>6.072943404997204</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:28:20.154728</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>17.94780154299951</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:01:09.468831</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 22)</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>20.13124113599997</v>
+      </c>
+      <c r="G26" t="n">
+        <v>22</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:26:25.510004</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>6.554649730001984</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:29:03.014644</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>20.23042048500065</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:01:09.468831</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 7)</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>30.89984609900011</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:27:36.633534</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>6.049241011998674</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:29:36.018999</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>14.15438628999982</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:28:11.995146</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>6.303271404998668</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:30:07.567358</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>14.06064980800147</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:28:50.105511</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>5.668358299000829</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:30:37.525788</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>11.65894129399749</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:29:29.601333</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>6.183931113999279</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:31:04.920495</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>12.2581570830007</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:30:02.376937</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>7.12968110699876</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:31:51.259423</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>15.94989597600215</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:30:32.122926</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>6.134777331000805</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:32:31.617178</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>16.91584824900201</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:31:00.989213</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>6.479192823000631</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:35:54.661968</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>16.36474248000013</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:31:45.450156</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>6.534823109999707</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:36:37.000132</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>21.52797504000046</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:32:27.670087</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>9.558821201000683</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:37:15.702678</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>17.71235919900209</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:33:15.600967</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>9.023647314999835</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:37:52.226616</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>14.37758300999849</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:35:46.943498</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>7.161070899001061</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:11:00.635840</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>11.97499336200053</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:36:28.548819</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>6.500482330997329</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:37:07.896621</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>6.344792412997776</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:37:46.502192</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>7.236187489997974</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:42:38.486038</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>6.856922298000427</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:11:00.554425</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>10.39790224299941</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:17:08.391051</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>7.020958000000974</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:22:12.580287</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>0.1523438369986252</v>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46">
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="J46" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>15.04</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>25.15</t>
+        </is>
+      </c>
+      <c r="I47" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>6.73</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>9.22</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>15.56</t>
+        </is>
+      </c>
+      <c r="I48" s="1" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>23.06</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>37.99</t>
+        </is>
+      </c>
+      <c r="I49" s="1" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>10.40</t>
+        </is>
+      </c>
+    </row>
+    <row r="50"/>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>Error Type</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>Error Message</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:56:53.043192</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise Callback</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Failed to execute pick and raise operation: Waypoint execution failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-07-08T22:56:53.065961</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Failed to pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:16:59.150607</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Add Package Callback</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Failed to find placement for package with ID 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:16:59.174089</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Unable to find a place for the package</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:26:59.288288</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Package height is too high. Measured 204 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:27:06.637060</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Package length is too long. Measured 414 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:42:46.228905</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Add Package Callback</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Failed to find placement for package with ID 37</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-07-08T23:42:46.248970</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Unable to find a place for the package</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:16:43.556644</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Package length is too long. Measured 410 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:17:16.528185</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Add Package Callback</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Failed to find placement for package with ID 38</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:17:16.552050</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Unable to find a place for the package</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:22:12.580287</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>No contours found</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:57:29.132885</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:57:29.138871</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Error message not found</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:57:29.145963</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 8</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:58:22.572326</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Failed to execute pick and place operation: Waypoint execution failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-07-09T00:58:22.579425</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 9</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:04:06.729963</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Failed to execute pick and place operation: Waypoint execution failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:04:06.741982</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 2</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:14:06.484565</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Failed to execute pick and place operation: Waypoint execution failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-07-09T01:14:06.501028</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 18</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="73"/>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Time Bins (s)</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>9.22-10.61</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>10.61-11.99</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>11.99-13.37</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>13.37-14.76</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>14.76-16.14</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>16.14-17.52</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>17.52-18.91</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>18.91-20.29</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>20.29-21.67</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>21.67-23.06</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85"/>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Time Bins (s)</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>15.56-17.81</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>17.81-20.05</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>20.05-22.29</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>22.29-24.53</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>24.53-26.78</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>26.78-29.02</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>29.02-31.26</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>31.26-33.50</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>33.50-35.75</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>35.75-37.99</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97"/>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Time Bins (s)</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>0.15-1.18</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>1.18-2.20</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2.20-3.23</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>3.23-4.25</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>4.25-5.28</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>5.28-6.30</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>6.30-7.32</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>7.32-8.35</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>8.35-9.37</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>9.37-10.40</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109"/>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Hour</t>
+        </is>
+      </c>
+      <c r="B110" s="1" t="inlineStr">
+        <is>
+          <t>Packages Retrieved</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-07-08 23:00</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-07-09 00:00</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-07-09 01:00</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Process new log data and update report
</commit_message>
<xml_diff>
--- a/master_report.xlsx
+++ b/master_report.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Day 2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Day 3" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Day 4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Day 5" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -186,12 +187,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$5</f>
+              <f>'Master Summary'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$C$2:$C$5</f>
+              <f>'Master Summary'!$C$2:$C$6</f>
             </numRef>
           </val>
         </ser>
@@ -218,12 +219,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$5</f>
+              <f>'Master Summary'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$D$2:$D$5</f>
+              <f>'Master Summary'!$D$2:$D$6</f>
             </numRef>
           </val>
         </ser>
@@ -250,12 +251,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$5</f>
+              <f>'Master Summary'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$E$2:$E$5</f>
+              <f>'Master Summary'!$E$2:$E$6</f>
             </numRef>
           </val>
         </ser>
@@ -1035,6 +1036,70 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 5'!B75</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 5'!$A$76:$A$85</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 5'!$B$76:$B$85</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
@@ -1079,12 +1144,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Master Summary'!$A$2:$A$5</f>
+              <f>'Master Summary'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Master Summary'!$J$2:$J$5</f>
+              <f>'Master Summary'!$J$2:$J$6</f>
             </numRef>
           </val>
         </ser>
@@ -1116,7 +1181,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Master Summary'!$K$2:$K$5</f>
+              <f>'Master Summary'!$K$2:$K$6</f>
             </numRef>
           </val>
         </ser>
@@ -1205,6 +1270,243 @@
     <legend>
       <legendPos val="r"/>
     </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 5'!B87</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 5'!$A$88:$A$97</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 5'!$B$88:$B$97</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 5'!B99</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 5'!$A$100:$A$109</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 5'!$B$100:$B$109</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Hourly Package Retrieval Throughput</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Day 5'!B111</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Day 5'!$A$112:$A$114</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Day 5'!$B$112:$B$114</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Hour of Day</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Packages Retrieved</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
@@ -1710,7 +2012,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>6</row>
+      <row>7</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -1732,7 +2034,7 @@
     <from>
       <col>9</col>
       <colOff>0</colOff>
-      <row>6</row>
+      <row>7</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="2700000"/>
@@ -2125,6 +2427,99 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>74</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>86</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>98</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>110</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2414,7 +2809,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2659,6 +3054,49 @@
       </c>
       <c r="M5" t="n">
         <v>0.2797005152777778</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-07-09</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>15.66</v>
+      </c>
+      <c r="D6" t="n">
+        <v>26.52</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7.97</v>
+      </c>
+      <c r="F6" t="n">
+        <v>33</v>
+      </c>
+      <c r="G6" t="n">
+        <v>41</v>
+      </c>
+      <c r="H6" t="n">
+        <v>28</v>
+      </c>
+      <c r="I6" t="n">
+        <v>39</v>
+      </c>
+      <c r="J6" t="n">
+        <v>36.09</v>
+      </c>
+      <c r="K6" t="n">
+        <v>27</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.7140406888888891</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.7758506075000001</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +3111,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2772,6 +3210,16 @@
           <t>Failed to pick and raise</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Failed to find packages with IDs: [X]</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Failed to find package</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -2922,6 +3370,49 @@
       </c>
       <c r="R5" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-07-09</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2</v>
+      </c>
+      <c r="T6" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -9053,52 +9544,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Event Label</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Event Label</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Package ID</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Event Label</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
@@ -10648,24 +11139,24 @@
     </row>
     <row r="45"/>
     <row r="46">
-      <c r="B46" s="1" t="inlineStr">
+      <c r="B46" s="2" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="E46" s="1" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
-      <c r="J46" s="1" t="inlineStr">
+      <c r="J46" t="inlineStr">
         <is>
           <t>Time (s)</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -10675,7 +11166,7 @@
           <t>15.04</t>
         </is>
       </c>
-      <c r="D47" s="1" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -10685,7 +11176,7 @@
           <t>25.15</t>
         </is>
       </c>
-      <c r="I47" s="1" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -10697,7 +11188,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
+      <c r="A48" s="2" t="inlineStr">
         <is>
           <t>Minimum</t>
         </is>
@@ -10707,7 +11198,7 @@
           <t>9.22</t>
         </is>
       </c>
-      <c r="D48" s="1" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Minimum</t>
         </is>
@@ -10717,7 +11208,7 @@
           <t>15.56</t>
         </is>
       </c>
-      <c r="I48" s="1" t="inlineStr">
+      <c r="I48" t="inlineStr">
         <is>
           <t>Minimum</t>
         </is>
@@ -10729,7 +11220,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
+      <c r="A49" s="2" t="inlineStr">
         <is>
           <t>Maximum</t>
         </is>
@@ -10739,7 +11230,7 @@
           <t>23.06</t>
         </is>
       </c>
-      <c r="D49" s="1" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Maximum</t>
         </is>
@@ -10749,7 +11240,7 @@
           <t>37.99</t>
         </is>
       </c>
-      <c r="I49" s="1" t="inlineStr">
+      <c r="I49" t="inlineStr">
         <is>
           <t>Maximum</t>
         </is>
@@ -10762,17 +11253,17 @@
     </row>
     <row r="50"/>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="B51" s="1" t="inlineStr">
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>Error Type</t>
         </is>
       </c>
-      <c r="C51" s="1" t="inlineStr">
+      <c r="C51" s="2" t="inlineStr">
         <is>
           <t>Error Message</t>
         </is>
@@ -11137,12 +11628,12 @@
     </row>
     <row r="73"/>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
+      <c r="A74" s="2" t="inlineStr">
         <is>
           <t>Time Bins (s)</t>
         </is>
       </c>
-      <c r="B74" s="1" t="inlineStr">
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -11250,12 +11741,12 @@
     </row>
     <row r="85"/>
     <row r="86">
-      <c r="A86" s="1" t="inlineStr">
+      <c r="A86" s="2" t="inlineStr">
         <is>
           <t>Time Bins (s)</t>
         </is>
       </c>
-      <c r="B86" s="1" t="inlineStr">
+      <c r="B86" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -11363,12 +11854,12 @@
     </row>
     <row r="97"/>
     <row r="98">
-      <c r="A98" s="1" t="inlineStr">
+      <c r="A98" s="2" t="inlineStr">
         <is>
           <t>Time Bins (s)</t>
         </is>
       </c>
-      <c r="B98" s="1" t="inlineStr">
+      <c r="B98" s="2" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
@@ -11476,12 +11967,12 @@
     </row>
     <row r="109"/>
     <row r="110">
-      <c r="A110" s="1" t="inlineStr">
+      <c r="A110" s="2" t="inlineStr">
         <is>
           <t>Hour</t>
         </is>
       </c>
-      <c r="B110" s="1" t="inlineStr">
+      <c r="B110" s="2" t="inlineStr">
         <is>
           <t>Packages Retrieved</t>
         </is>
@@ -11522,4 +12013,2497 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Event Label</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Event Label</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Package ID</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Event Label</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:00:23.881885</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>10.31653603899997</v>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:52:03.631473</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 7)</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>27.98937887700004</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:00:23.121547</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>9.405105400000025</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:01:22.644883</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>12.844262254</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:52:03.631473</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 2)</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>18.08887379199996</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:01:18.072921</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>8.157038041999954</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:01:47.470773</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>9.834047141000042</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:55:44.296723</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 9)</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>23.54727898700003</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:01:47.037100</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>9.247409285999993</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:03:06.839028</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>12.01649419600005</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:58:08.734588</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 12)</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>32.01135078800053</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:03:03.638161</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>6.897099805999915</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:03:44.498745</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>15.33017479699993</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:58:08.734588</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 1)</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>32.77284770299957</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:03:37.617454</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>6.614939216000039</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:04:35.903116</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>14.92194235099998</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:59:10.513957</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 6)</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>27.11092348599959</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:04:28.762056</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>6.161488025999915</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:05:51.305490</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>14.80966519399999</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-07-09T18:00:12.422584</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 5)</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>23.47054978399956</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:05:45.443970</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>7.119074510999781</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:06:51.824195</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>14.28557416100011</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:03:35.720809</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 4)</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>29.09976904599989</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:06:45.293099</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>6.159382433000019</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:07:31.314849</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>15.48240047699983</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:07:28.007002</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 2)</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>24.51250604400047</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:07:24.072217</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>6.417692975000136</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:27:06.553309</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>20.73392708099982</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:12:56.448087</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 6)</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>24.95451355200021</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:08:06.371557</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>0.1080534509999325</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:30:32.672788</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>13.12091660999977</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:12:56.448087</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 9)</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>30.02236789700055</v>
+      </c>
+      <c r="G12" t="n">
+        <v>9</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:26:59.647686</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>6.451890132000244</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:31:07.543978</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>16.05095809200066</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:14:37.093266</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 19)</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>24.42882732700036</v>
+      </c>
+      <c r="G13" t="n">
+        <v>19</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:30:30.101595</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>8.816499478999503</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:31:46.729156</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>17.94641303800017</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:14:37.093266</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 5)</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>36.19164207799986</v>
+      </c>
+      <c r="G14" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:31:01.738214</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>8.540726980000727</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:32:27.537991</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>20.56321398599994</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:14:37.093266</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 15)</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>25.41339611600051</v>
+      </c>
+      <c r="G15" t="n">
+        <v>15</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:31:37.819749</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>7.299677785000313</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:33:18.637330</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>25.7929218700001</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:18:09.189021</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 17)</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>23.76677668100001</v>
+      </c>
+      <c r="G16" t="n">
+        <v>17</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:32:20.341560</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>11.75148576600077</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:33:55.321304</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>16.62895203100015</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:20:06.181633</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 7)</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>31.09475319400008</v>
+      </c>
+      <c r="G17" t="n">
+        <v>7</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:33:07.793293</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>7.708521808000114</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:34:33.378316</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>16.69303597800081</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:20:06.181633</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 23)</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>22.24986878300024</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:33:49.288918</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>9.006529381000291</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:35:11.320238</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>14.20121001000007</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:22:23.400353</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 14)</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>31.73017048200018</v>
+      </c>
+      <c r="G19" t="n">
+        <v>14</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:34:30.067643</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>11.63869443600015</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:35:36.659589</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>10.04445122899961</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:22:23.400353</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 1)</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>27.51738054499947</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:35:05.386697</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>8.106902147000255</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:36:05.824446</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>10.70958015799988</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:22:23.400353</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 8)</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>17.82745720999992</v>
+      </c>
+      <c r="G21" t="n">
+        <v>8</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:35:35.226695</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>8.520435885000552</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:36:31.723505</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>10.81042264499956</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:26:44.935612</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 3)</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>26.06856092599992</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:36:07.336123</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>12.07209446199977</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:37:03.480749</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>15.64828218299954</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:28:01.722603</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 12)</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>23.45742417600013</v>
+      </c>
+      <c r="G23" t="n">
+        <v>12</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:36:29.537481</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>8.480712200000198</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:37:41.568775</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>19.93703968200043</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:29:56.057016</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 10)</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>30.42259148599987</v>
+      </c>
+      <c r="G24" t="n">
+        <v>10</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:36:57.813144</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>6.521772070000225</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:38:38.847701</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>15.09483054300017</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:31:50.204802</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 13)</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>27.66220764100035</v>
+      </c>
+      <c r="G25" t="n">
+        <v>13</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:37:32.893677</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>9.810703275999913</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:39:06.680216</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>16.08665306400053</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:32:35.149130</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 21)</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>26.00436577399887</v>
+      </c>
+      <c r="G26" t="n">
+        <v>21</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:38:33.987930</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>8.629125122000005</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:41:01.983415</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>17.74713734099987</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:33:48.306727</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 24)</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>28.95819014299923</v>
+      </c>
+      <c r="G27" t="n">
+        <v>24</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:38:59.265073</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>6.954240297000069</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:41:59.809814</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>15.86082442799943</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:38:27.284214</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 20)</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>28.07570936999946</v>
+      </c>
+      <c r="G28" t="n">
+        <v>20</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:39:29.977912</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>7.272197137000148</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:42:38.312829</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>18.52679474199977</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:41:59.991885</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Individual Retrieval (ID: 11)</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>18.21678022199922</v>
+      </c>
+      <c r="G29" t="n">
+        <v>11</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:40:17.407669</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>6.873431026000617</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:43:14.038222</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>16.91407942499973</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:40:55.082577</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>7.356497611000123</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:43:48.315982</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>14.85157977299968</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:41:52.569669</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>6.921981114000118</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:45:06.857992</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>15.41171263100023</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:42:31.549409</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>8.263683973000298</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:45:47.677996</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>16.40907521200006</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:43:08.035381</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>9.204706790000273</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:46:40.547844</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>21.12880615800077</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:43:40.411913</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>6.803173390999291</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:45:03.272091</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>10.16644128699954</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:45:40.087592</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>7.225754842000242</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:46:28.717921</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>7.40263581399995</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:56:27.405597</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>10.9151503310004</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:56:48.251831</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>7.771012766999775</v>
+      </c>
+    </row>
+    <row r="40"/>
+    <row r="41">
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+      <c r="J41" s="1" t="inlineStr">
+        <is>
+          <t>Time (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>15.66</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>26.52</t>
+        </is>
+      </c>
+      <c r="I42" s="1" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>7.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>9.83</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>17.83</t>
+        </is>
+      </c>
+      <c r="I43" s="1" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>25.79</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>36.19</t>
+        </is>
+      </c>
+      <c r="I44" s="1" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>12.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>Error Type</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>Error Message</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:01:47.037100</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Failed to extract address using GPT query</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:04:12.589235</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Package length is too long. Measured 438 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:05:01.688080</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Package length is too long. Measured 411 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:08:06.371557</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>No contours found</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-07-09T17:45:36.009750</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Failed to find packages with IDs: [10]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-07-09T18:02:26.276053</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-07-09T18:02:26.277270</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Error message not found</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-07-09T18:02:26.285881</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 4</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-07-09T18:03:36.485227</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Find Package Callback</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Failed to find package</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-07-09T18:03:36.491422</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Failed to find package</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:36:07.336123</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Failed to extract address using GPT query</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:37:32.893677</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Read Label Callback</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Failed to extract address using GPT query</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:39:40.083563</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Package height when sagging is too high. Measured 192 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:40:28.663328</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:40:28.673805</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Package height when sagging is too high. Measured 285 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:52:36.900737</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Package height is too high. Measured 215 mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:56:32.092396</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:56:32.103587</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Sag height was not found. Did package fully clear the platform?</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:56:56.326403</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-07-09T20:56:56.350654</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Conveyable Stow</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Sag height was not found. Did package fully clear the platform?</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:14:57.673519</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Failed to find packages with IDs: [9]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:36:10.061029</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:36:10.068756</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Error message not found</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:36:10.076362</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 22</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:41:01.897946</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Execute Pick and Raise</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Vacuum not achieved, aborting pick and raise</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:41:01.900418</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Execute Pick and Place Callback</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Error message not found</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-07-09T21:41:01.993078</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Retrieve Packages Callback: 18</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Failed in attempt to pick and place: Failed to pick and place</t>
+        </is>
+      </c>
+    </row>
+    <row r="74"/>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Time Bins (s)</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>9.83-11.43</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>11.43-13.03</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>13.03-14.62</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>14.62-16.22</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>16.22-17.81</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>17.81-19.41</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>19.41-21.01</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>21.01-22.60</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>22.60-24.20</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>24.20-25.79</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86"/>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Time Bins (s)</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>17.83-19.66</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>19.66-21.50</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>21.50-23.34</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>23.34-25.17</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>25.17-27.01</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>27.01-28.85</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>28.85-30.68</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>30.68-32.52</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>32.52-34.36</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>34.36-36.19</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98"/>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Time Bins (s)</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>0.11-1.30</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>1.30-2.50</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2.50-3.70</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>3.70-4.89</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>4.89-6.09</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>6.09-7.29</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>7.29-8.48</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>8.48-9.68</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>9.68-10.88</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>10.88-12.07</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110"/>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Hour</t>
+        </is>
+      </c>
+      <c r="B111" s="1" t="inlineStr">
+        <is>
+          <t>Packages Retrieved</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-07-09 17:00</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-07-09 18:00</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-07-09 21:00</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new tab for benchmark, not compatible with new retrieve logs
</commit_message>
<xml_diff>
--- a/master_report.xlsx
+++ b/master_report.xlsx
@@ -8,12 +8,12 @@
   </bookViews>
   <sheets>
     <sheet name="Master Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Error Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Day 1" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Day 2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Day 3" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Day 4" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Day 5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Day 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Day 2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Day 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Day 4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Day 5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Error Summary" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Day 6" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
@@ -3463,279 +3463,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Day</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Uncategorized Error</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Vision: Address Extraction Failed</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Vision: Package Not Found</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Vision: Sag Height Not Found</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Packing: Placement Failure</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>End Effector: Vacuum Failure</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Physical Constraints: Package Dimension Error</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Motion: Pick/Place Execution Failed</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Unknown: No Error Message</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Motion: Pick/Raise Execution Failed</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-07-03</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>22</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-07-07</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>6</v>
-      </c>
-      <c r="G3" t="n">
-        <v>14</v>
-      </c>
-      <c r="I3" t="n">
-        <v>7</v>
-      </c>
-      <c r="J3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-07-08</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-07-08</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" t="n">
-        <v>7</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-07-09</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3</v>
-      </c>
-      <c r="J6" t="n">
-        <v>3</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2025-07-10</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>4</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5093,7 +4820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7918,7 +7645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9329,7 +9056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -11800,7 +11527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -14230,6 +13957,279 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Uncategorized Error</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Vision: Address Extraction Failed</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Vision: Package Not Found</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Vision: Sag Height Not Found</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Packing: Placement Failure</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>End Effector: Vacuum Failure</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Physical Constraints: Package Dimension Error</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Motion: Pick/Place Execution Failed</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Unknown: No Error Message</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Motion: Pick/Raise Execution Failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-07-03</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-07-07</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-07-08</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-07-08</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-07-09</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-07-10</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>